<commit_message>
Refactor fixes and testing
</commit_message>
<xml_diff>
--- a/History/CHRNE_HARP_hist.xlsx
+++ b/History/CHRNE_HARP_hist.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
         <v>6</v>
-      </c>
-      <c r="C8" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final refactoring and renaming
</commit_message>
<xml_diff>
--- a/History/CHRNE_HARP_hist.xlsx
+++ b/History/CHRNE_HARP_hist.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>